<commit_message>
ms bevs recco 1
</commit_message>
<xml_diff>
--- a/myapp/cert_templates/Agreement_Certificate.xlsx
+++ b/myapp/cert_templates/Agreement_Certificate.xlsx
@@ -5,26 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\thesis_osa\myapp\cert_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3D213F-7505-4B75-AA57-DAA2A103C082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF9A94E-A260-41B7-8B10-A4FA5F7B5A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Agreement Certificate" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="date">inputs!$B$5</definedName>
-    <definedName name="end_date">inputs!$B$7</definedName>
-    <definedName name="hours">inputs!$B$9</definedName>
-    <definedName name="osa_head">inputs!$B$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$1:$18</definedName>
-    <definedName name="program">inputs!$B$4</definedName>
-    <definedName name="start_date">inputs!$B$6</definedName>
-    <definedName name="student_id">inputs!$B$3</definedName>
+    <definedName name="osa_head">inputs!$B$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Agreement Certificate'!$1:$21</definedName>
+    <definedName name="program">inputs!$B$3</definedName>
     <definedName name="student_name">inputs!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -48,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -62,12 +57,6 @@
     <t>Lord Jaisson Riberal</t>
   </si>
   <si>
-    <t>student_id</t>
-  </si>
-  <si>
-    <t>TUPC-22-0374</t>
-  </si>
-  <si>
     <t>program</t>
   </si>
   <si>
@@ -83,9 +72,6 @@
     <t>TECHNOLOGICAL UNIVERSITY OF THE PHILIPPINES</t>
   </si>
   <si>
-    <t>hours</t>
-  </si>
-  <si>
     <t>Head, Office of Student Affairs</t>
   </si>
   <si>
@@ -93,21 +79,6 @@
   </si>
   <si>
     <t xml:space="preserve">                   CAVITE CAMPUS</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>November 10. 2025</t>
-  </si>
-  <si>
-    <t>November 20, 2025</t>
   </si>
   <si>
     <t>COMMUNITY SERVICE COMPLETION AGREEMENT</t>
@@ -200,51 +171,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -605,46 +568,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5">
-        <v>45699</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -656,7 +579,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -671,86 +594,80 @@
   <sheetData>
     <row r="1" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="12" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="str">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="str">
         <f xml:space="preserve"> "I " &amp; student_name &amp; " from the " &amp; program &amp; " program, understand that I must complete all pending community service hours before the end of the current semester or before applying for clearance for any academic credential. Failure to comply may result in delayed or denied clearance."</f>
         <v>I Lord Jaisson Riberal from the BET-COET program, understand that I must complete all pending community service hours before the end of the current semester or before applying for clearance for any academic credential. Failure to comply may result in delayed or denied clearance.</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" s="12" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:4" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="15" t="str">
+      <c r="B16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4" t="str">
         <f>osa_head</f>
         <v>Beverly M. de Vega</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-    </row>
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2"/>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2"/>

</xml_diff>